<commit_message>
refactor: refactored code base
</commit_message>
<xml_diff>
--- a/data/exam_input_data_test.xlsx
+++ b/data/exam_input_data_test.xlsx
@@ -438,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,6 +449,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -531,6 +535,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,13 +596,13 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="n">
@@ -611,13 +619,13 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="n">
@@ -634,13 +642,13 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="n">
@@ -657,13 +665,13 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="n">
@@ -680,13 +688,13 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="n">
@@ -703,16 +711,16 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="n">
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="n">
         <v>800</v>
       </c>
       <c r="F7" s="2" t="n">
@@ -726,16 +734,16 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5" t="n">
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="n">
         <v>107</v>
       </c>
       <c r="F8" s="2" t="n">
@@ -749,16 +757,16 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="n">
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="n">
         <v>900</v>
       </c>
       <c r="F9" s="2" t="n">
@@ -772,16 +780,16 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5" t="n">
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="n">
         <v>120</v>
       </c>
       <c r="F10" s="2" t="n">
@@ -795,16 +803,16 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="5" t="n">
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6" t="n">
         <v>850</v>
       </c>
       <c r="F11" s="2" t="n">
@@ -818,16 +826,16 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="n">
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="n">
         <v>100</v>
       </c>
       <c r="F12" s="2" t="n">
@@ -841,13 +849,13 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="n">
@@ -864,16 +872,16 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5" t="n">
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="n">
         <v>790</v>
       </c>
       <c r="F14" s="2" t="n">
@@ -887,16 +895,16 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="5" t="n">
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="n">
         <v>174</v>
       </c>
       <c r="F15" s="2" t="n">
@@ -910,16 +918,16 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="5" t="n">
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="n">
         <v>95</v>
       </c>
       <c r="F16" s="2" t="n">
@@ -933,16 +941,16 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="5" t="n">
+      <c r="D17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="n">
         <v>108</v>
       </c>
       <c r="F17" s="2" t="n">
@@ -956,16 +964,16 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="5" t="n">
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6" t="n">
         <v>60</v>
       </c>
       <c r="F18" s="2" t="n">
@@ -979,16 +987,16 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="5" t="n">
+      <c r="D19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="2" t="n">
@@ -1002,16 +1010,16 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5" t="n">
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="6" t="n">
         <v>32</v>
       </c>
       <c r="F20" s="2" t="n">
@@ -1025,16 +1033,16 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="n">
+      <c r="D21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6" t="n">
         <v>15</v>
       </c>
       <c r="F21" s="2" t="n">
@@ -1048,16 +1056,16 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="5" t="n">
+      <c r="D22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6" t="n">
         <v>12</v>
       </c>
       <c r="F22" s="2" t="n">
@@ -1071,13 +1079,13 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="n">
@@ -1094,16 +1102,16 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="5" t="n">
+      <c r="D24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="6" t="n">
         <v>87</v>
       </c>
       <c r="F24" s="2" t="n">
@@ -1117,16 +1125,16 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="5" t="n">
+      <c r="D25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="6" t="n">
         <v>171</v>
       </c>
       <c r="F25" s="2" t="n">
@@ -1140,16 +1148,16 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="5" t="n">
+      <c r="D26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="6" t="n">
         <v>80</v>
       </c>
       <c r="F26" s="2" t="n">
@@ -1163,16 +1171,16 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="5" t="n">
+      <c r="D27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="6" t="n">
         <v>9</v>
       </c>
       <c r="F27" s="2" t="n">
@@ -1186,16 +1194,16 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="5" t="n">
+      <c r="D28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="6" t="n">
         <v>55</v>
       </c>
       <c r="F28" s="2" t="n">
@@ -1209,16 +1217,16 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="5" t="n">
+      <c r="D29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="6" t="n">
         <v>29</v>
       </c>
       <c r="F29" s="2" t="n">
@@ -1232,16 +1240,16 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="5" t="n">
+      <c r="D30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="6" t="n">
         <v>112</v>
       </c>
       <c r="F30" s="2" t="n">
@@ -1255,16 +1263,16 @@
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5" t="n">
+      <c r="D31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="6" t="n">
         <v>100</v>
       </c>
       <c r="F31" s="2" t="n">
@@ -1278,16 +1286,16 @@
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="5" t="n">
+      <c r="D32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="6" t="n">
         <v>850</v>
       </c>
       <c r="F32" s="2" t="n">
@@ -1301,16 +1309,16 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="5" t="n">
+      <c r="D33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F33" s="2" t="n">
@@ -1324,16 +1332,16 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="5" t="n">
+      <c r="D34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="6" t="n">
         <v>38</v>
       </c>
       <c r="F34" s="2" t="n">
@@ -1347,13 +1355,13 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -1370,16 +1378,16 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="5" t="n">
+      <c r="D36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="6" t="n">
         <v>29</v>
       </c>
       <c r="F36" s="2" t="n">
@@ -1393,16 +1401,16 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="5" t="n">
+      <c r="D37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="6" t="n">
         <v>19</v>
       </c>
       <c r="F37" s="2" t="n">
@@ -1416,16 +1424,16 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="5" t="n">
+      <c r="D38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="6" t="n">
         <v>4</v>
       </c>
       <c r="F38" s="2" t="n">
@@ -1439,16 +1447,16 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="5" t="n">
+      <c r="D39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="6" t="n">
         <v>182</v>
       </c>
       <c r="F39" s="2" t="n">
@@ -1513,7 +1521,7 @@
       <c r="B2" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <v>43926</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1530,7 +1538,7 @@
       <c r="B3" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="7" t="n">
         <v>43926</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -1547,7 +1555,7 @@
       <c r="B4" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <v>43926</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1564,7 +1572,7 @@
       <c r="B5" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <v>43956</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1581,7 +1589,7 @@
       <c r="B6" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>43956</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -1598,7 +1606,7 @@
       <c r="B7" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="7" t="n">
         <v>43956</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1615,7 +1623,7 @@
       <c r="B8" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="7" t="n">
         <v>43987</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1632,7 +1640,7 @@
       <c r="B9" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="7" t="n">
         <v>43987</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1649,7 +1657,7 @@
       <c r="B10" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="7" t="n">
         <v>43987</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1666,7 +1674,7 @@
       <c r="B11" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="7" t="n">
         <v>44017</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1683,7 +1691,7 @@
       <c r="B12" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="7" t="n">
         <v>44017</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1700,7 +1708,7 @@
       <c r="B13" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="7" t="n">
         <v>44017</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1717,7 +1725,7 @@
       <c r="B14" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="7" t="n">
         <v>44048</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1734,7 +1742,7 @@
       <c r="B15" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="7" t="n">
         <v>44048</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -1751,7 +1759,7 @@
       <c r="B16" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="7" t="n">
         <v>44048</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1768,7 +1776,7 @@
       <c r="B17" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="7" t="n">
         <v>44140</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1785,7 +1793,7 @@
       <c r="B18" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="7" t="n">
         <v>44140</v>
       </c>
       <c r="D18" s="0" t="s">
@@ -1802,7 +1810,7 @@
       <c r="B19" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C19" s="7" t="n">
         <v>44140</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1819,7 +1827,7 @@
       <c r="B20" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="7" t="n">
         <v>44170</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1836,7 +1844,7 @@
       <c r="B21" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C21" s="6" t="n">
+      <c r="C21" s="7" t="n">
         <v>44170</v>
       </c>
       <c r="D21" s="0" t="s">
@@ -1853,7 +1861,7 @@
       <c r="B22" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C22" s="6" t="n">
+      <c r="C22" s="7" t="n">
         <v>44170</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2195,7 +2203,7 @@
   <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2211,67 +2219,67 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="14" t="n">
         <v>1630</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="15" t="n">
         <v>850</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="16" t="n">
-        <v>1630</v>
-      </c>
-      <c r="D5" s="17" t="n">
+      <c r="C5" s="17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="19" t="n">
         <f aca="false">E4+D4</f>
         <v>2480</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="20" t="n">
-        <v>850</v>
-      </c>
-      <c r="D6" s="21" t="n">
-        <v>2480</v>
-      </c>
-      <c r="E6" s="22" t="n">
+      <c r="C6" s="21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2307,178 +2315,178 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Distance back to back penalty function
</commit_message>
<xml_diff>
--- a/data/exam_input_data_test.xlsx
+++ b/data/exam_input_data_test.xlsx
@@ -438,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,10 +449,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -535,10 +531,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,13 +588,13 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="n">
@@ -619,13 +611,13 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="n">
@@ -642,13 +634,13 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="n">
@@ -665,13 +657,13 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="n">
@@ -688,13 +680,13 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="n">
@@ -711,16 +703,16 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="n">
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>800</v>
       </c>
       <c r="F7" s="2" t="n">
@@ -734,16 +726,16 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="n">
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>107</v>
       </c>
       <c r="F8" s="2" t="n">
@@ -757,16 +749,16 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6" t="n">
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>900</v>
       </c>
       <c r="F9" s="2" t="n">
@@ -780,16 +772,16 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="6" t="n">
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>120</v>
       </c>
       <c r="F10" s="2" t="n">
@@ -803,16 +795,16 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="6" t="n">
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="n">
         <v>850</v>
       </c>
       <c r="F11" s="2" t="n">
@@ -826,16 +818,16 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="6" t="n">
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="n">
         <v>100</v>
       </c>
       <c r="F12" s="2" t="n">
@@ -849,13 +841,13 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="n">
@@ -872,16 +864,16 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="6" t="n">
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5" t="n">
         <v>790</v>
       </c>
       <c r="F14" s="2" t="n">
@@ -895,16 +887,16 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="6" t="n">
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5" t="n">
         <v>174</v>
       </c>
       <c r="F15" s="2" t="n">
@@ -918,16 +910,16 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="6" t="n">
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="n">
         <v>95</v>
       </c>
       <c r="F16" s="2" t="n">
@@ -941,16 +933,16 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="6" t="n">
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="n">
         <v>108</v>
       </c>
       <c r="F17" s="2" t="n">
@@ -964,16 +956,16 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="6" t="n">
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5" t="n">
         <v>60</v>
       </c>
       <c r="F18" s="2" t="n">
@@ -987,16 +979,16 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="n">
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="2" t="n">
@@ -1010,16 +1002,16 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="6" t="n">
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <v>32</v>
       </c>
       <c r="F20" s="2" t="n">
@@ -1033,16 +1025,16 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="6" t="n">
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="5" t="n">
         <v>15</v>
       </c>
       <c r="F21" s="2" t="n">
@@ -1056,16 +1048,16 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="6" t="n">
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="5" t="n">
         <v>12</v>
       </c>
       <c r="F22" s="2" t="n">
@@ -1079,13 +1071,13 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="n">
@@ -1102,16 +1094,16 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="6" t="n">
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="5" t="n">
         <v>87</v>
       </c>
       <c r="F24" s="2" t="n">
@@ -1125,16 +1117,16 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="6" t="n">
+      <c r="D25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="5" t="n">
         <v>171</v>
       </c>
       <c r="F25" s="2" t="n">
@@ -1148,16 +1140,16 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="6" t="n">
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="5" t="n">
         <v>80</v>
       </c>
       <c r="F26" s="2" t="n">
@@ -1171,16 +1163,16 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="6" t="n">
+      <c r="D27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="n">
         <v>9</v>
       </c>
       <c r="F27" s="2" t="n">
@@ -1194,16 +1186,16 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="6" t="n">
+      <c r="D28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="5" t="n">
         <v>55</v>
       </c>
       <c r="F28" s="2" t="n">
@@ -1217,16 +1209,16 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="6" t="n">
+      <c r="D29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="5" t="n">
         <v>29</v>
       </c>
       <c r="F29" s="2" t="n">
@@ -1240,16 +1232,16 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="6" t="n">
+      <c r="D30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="5" t="n">
         <v>112</v>
       </c>
       <c r="F30" s="2" t="n">
@@ -1263,16 +1255,16 @@
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="6" t="n">
+      <c r="D31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="5" t="n">
         <v>100</v>
       </c>
       <c r="F31" s="2" t="n">
@@ -1286,16 +1278,16 @@
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="6" t="n">
+      <c r="D32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5" t="n">
         <v>850</v>
       </c>
       <c r="F32" s="2" t="n">
@@ -1309,16 +1301,16 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="6" t="n">
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="5" t="n">
         <v>6</v>
       </c>
       <c r="F33" s="2" t="n">
@@ -1332,16 +1324,16 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="6" t="n">
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5" t="n">
         <v>38</v>
       </c>
       <c r="F34" s="2" t="n">
@@ -1355,13 +1347,13 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -1378,16 +1370,16 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="6" t="n">
+      <c r="D36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="5" t="n">
         <v>29</v>
       </c>
       <c r="F36" s="2" t="n">
@@ -1401,16 +1393,16 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="6" t="n">
+      <c r="D37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="5" t="n">
         <v>19</v>
       </c>
       <c r="F37" s="2" t="n">
@@ -1424,16 +1416,16 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="6" t="n">
+      <c r="D38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="5" t="n">
         <v>4</v>
       </c>
       <c r="F38" s="2" t="n">
@@ -1447,16 +1439,16 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="6" t="n">
+      <c r="D39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="5" t="n">
         <v>182</v>
       </c>
       <c r="F39" s="2" t="n">
@@ -1521,7 +1513,7 @@
       <c r="B2" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="6" t="n">
         <v>43926</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1538,7 +1530,7 @@
       <c r="B3" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>43926</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -1555,7 +1547,7 @@
       <c r="B4" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="6" t="n">
         <v>43926</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1572,7 +1564,7 @@
       <c r="B5" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>43956</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1589,7 +1581,7 @@
       <c r="B6" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="6" t="n">
         <v>43956</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -1606,7 +1598,7 @@
       <c r="B7" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>43956</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1623,7 +1615,7 @@
       <c r="B8" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>43987</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1640,7 +1632,7 @@
       <c r="B9" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="6" t="n">
         <v>43987</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1657,7 +1649,7 @@
       <c r="B10" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="6" t="n">
         <v>43987</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1674,7 +1666,7 @@
       <c r="B11" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="6" t="n">
         <v>44017</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1691,7 +1683,7 @@
       <c r="B12" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="6" t="n">
         <v>44017</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1708,7 +1700,7 @@
       <c r="B13" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>44017</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1725,7 +1717,7 @@
       <c r="B14" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="6" t="n">
         <v>44048</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1742,7 +1734,7 @@
       <c r="B15" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="6" t="n">
         <v>44048</v>
       </c>
       <c r="D15" s="0" t="s">
@@ -1759,7 +1751,7 @@
       <c r="B16" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>44048</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1776,7 +1768,7 @@
       <c r="B17" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="6" t="n">
         <v>44140</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1793,7 +1785,7 @@
       <c r="B18" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="6" t="n">
         <v>44140</v>
       </c>
       <c r="D18" s="0" t="s">
@@ -1810,7 +1802,7 @@
       <c r="B19" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="6" t="n">
         <v>44140</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1827,7 +1819,7 @@
       <c r="B20" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="6" t="n">
         <v>44170</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1844,7 +1836,7 @@
       <c r="B21" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="6" t="n">
         <v>44170</v>
       </c>
       <c r="D21" s="0" t="s">
@@ -1861,7 +1853,7 @@
       <c r="B22" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="6" t="n">
         <v>44170</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2219,67 +2211,67 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="13" t="n">
+      <c r="C4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="13" t="n">
         <v>1630</v>
       </c>
-      <c r="E4" s="15" t="n">
+      <c r="E4" s="14" t="n">
         <v>850</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="17" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="18" t="n">
+      <c r="C5" s="16" t="n">
+        <v>1630</v>
+      </c>
+      <c r="D5" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="19" t="n">
+      <c r="E5" s="18" t="n">
         <f aca="false">E4+D4</f>
         <v>2480</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="21" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="22" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="23" t="n">
+      <c r="C6" s="20" t="n">
+        <v>850</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>2480</v>
+      </c>
+      <c r="E6" s="22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2315,178 +2307,178 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="n">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="n">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>